<commit_message>
Cambios en modelos, descripcion a clase
</commit_message>
<xml_diff>
--- a/Archivos extras/Tablas modelos.xlsx
+++ b/Archivos extras/Tablas modelos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Estudios\Desarrollo de Software\3er año-2021\Prácticas Profesionalizantes III\Archivos fuera del repositorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Estudios\Desarrollo de Software\3ero-2021\Practicas Profesionalizantes III\Ateneo\Archivos extras\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC1F8CB-A7AD-42D0-8C5C-B72375CBA781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEDB7828-5D55-4669-91D3-4F618D3A2D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
   <si>
     <t>Profesor</t>
   </si>
@@ -178,6 +178,12 @@
   </si>
   <si>
     <t>boolean</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>string</t>
   </si>
 </sst>
 </file>
@@ -369,91 +375,91 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -739,7 +745,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,13 +753,13 @@
     <col min="1" max="1" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="35.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6.140625" style="1" bestFit="1" customWidth="1"/>
@@ -762,40 +768,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="33"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="19"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="42"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="16"/>
       <c r="G3" s="2"/>
-      <c r="I3" s="39" t="s">
+      <c r="I3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="41"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="27"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -880,14 +886,14 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="15"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="14"/>
       <c r="G7" s="9" t="s">
         <v>17</v>
       </c>
@@ -954,20 +960,20 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="28" t="s">
+      <c r="B11" s="29"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="15"/>
+      <c r="F11" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="30"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="42"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -979,22 +985,25 @@
       <c r="C12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="D12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="G12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="H12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="I12" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="J12" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="K12" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1008,38 +1017,41 @@
       <c r="C13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="D13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="G13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="H13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="I13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="J13" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="K13" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="27"/>
-      <c r="F15" s="19" t="s">
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="39"/>
+      <c r="F15" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="21"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="33"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
@@ -1094,12 +1106,12 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="24"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="36"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
@@ -1131,15 +1143,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="F11:K11"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="I3:N3"/>
     <mergeCell ref="A11:C11"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="E11:J11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>